<commit_message>
Session 2 and syllabus as a Readme file
</commit_message>
<xml_diff>
--- a/Training_Session_1/data/PRRS.xlsx
+++ b/Training_Session_1/data/PRRS.xlsx
@@ -36367,8 +36367,8 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AC53A90F68723D43865193287DBF125B" ma:contentTypeVersion="11" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="6d778c7599711c2b95c4859d4bb99a6c">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="39cfa7bf-be57-4825-ad81-4fa2c3988a7d" xmlns:ns3="609b3323-4b9d-43ca-b8cd-8ed7d7422988" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7f229267c19874a2a11b6278b017a4d4" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AC53A90F68723D43865193287DBF125B" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b951b4138421c1f6d18a2c1353684aac">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="39cfa7bf-be57-4825-ad81-4fa2c3988a7d" xmlns:ns3="609b3323-4b9d-43ca-b8cd-8ed7d7422988" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dab20cd784e680407d684fca2e46b6f9" ns2:_="" ns3:_="">
     <xsd:import namespace="39cfa7bf-be57-4825-ad81-4fa2c3988a7d"/>
     <xsd:import namespace="609b3323-4b9d-43ca-b8cd-8ed7d7422988"/>
     <xsd:element name="properties">
@@ -36447,7 +36447,7 @@
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="609b3323-4b9d-43ca-b8cd-8ed7d7422988" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="13" nillable="true" ma:displayName="Partagé avec" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="13" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -36466,7 +36466,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="14" nillable="true" ma:displayName="Partagé avec détails" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="14" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -36483,8 +36483,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Type de contenu"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titre"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -36591,20 +36591,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76F10877-0E5E-42BA-B188-E5865C8EE889}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="39cfa7bf-be57-4825-ad81-4fa2c3988a7d"/>
-    <ds:schemaRef ds:uri="609b3323-4b9d-43ca-b8cd-8ed7d7422988"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B105AF0-B7A3-4FEB-8ED6-F1A72E81BE9A}"/>
 </file>
</xml_diff>